<commit_message>
working program! gets tweet and plots mood over time
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14720" yWindow="3720" windowWidth="12200" windowHeight="11280" tabRatio="500"/>
+    <workbookView xWindow="16400" yWindow="6360" windowWidth="12200" windowHeight="11280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Word</t>
   </si>
@@ -30,64 +30,61 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>Neutral</t>
-  </si>
-  <si>
-    <t>HELLO</t>
-  </si>
-  <si>
-    <t>GOODBYE</t>
-  </si>
-  <si>
-    <t>GOOD</t>
-  </si>
-  <si>
-    <t>BAD</t>
-  </si>
-  <si>
-    <t>SAD</t>
-  </si>
-  <si>
-    <t>HURT</t>
-  </si>
-  <si>
-    <t>ALONE</t>
-  </si>
-  <si>
-    <t>SMILE</t>
-  </si>
-  <si>
-    <t>HAPPY</t>
-  </si>
-  <si>
-    <t>LOVE</t>
-  </si>
-  <si>
-    <t>ENJOY</t>
-  </si>
-  <si>
-    <t>LIKE</t>
-  </si>
-  <si>
-    <t>LIKED</t>
-  </si>
-  <si>
-    <t>PIZZA</t>
-  </si>
-  <si>
-    <t>FORCE</t>
-  </si>
-  <si>
-    <t>ANNOY</t>
-  </si>
-  <si>
-    <t>CAN'T</t>
-  </si>
-  <si>
-    <t>BROKEN</t>
-  </si>
-  <si>
-    <t>FIX</t>
+    <t>love</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>healthy</t>
+  </si>
+  <si>
+    <t>animals</t>
+  </si>
+  <si>
+    <t>late</t>
+  </si>
+  <si>
+    <t>sorry</t>
+  </si>
+  <si>
+    <t>accidents</t>
+  </si>
+  <si>
+    <t>awesome</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>proud</t>
+  </si>
+  <si>
+    <t>laughed</t>
+  </si>
+  <si>
+    <t>cried</t>
+  </si>
+  <si>
+    <t>inconvenience</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>old</t>
   </si>
 </sst>
 </file>
@@ -456,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,11 +471,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -486,27 +480,21 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -516,25 +504,19 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -544,11 +526,8 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -558,11 +537,8 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -572,11 +548,8 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -586,11 +559,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -600,11 +570,8 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -614,11 +581,8 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -628,25 +592,19 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -656,91 +614,70 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
         <v>0</v>
       </c>
     </row>

</xml_diff>